<commit_message>
utworzenie 4 arkuszy na kazdy tydzien prac
</commit_message>
<xml_diff>
--- a/backlog.xlsx
+++ b/backlog.xlsx
@@ -8,12 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stasz\mistrz_klawiatury\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EE24EF2E-4F5C-44E6-AE64-A774CE8CECF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65C2F86E-0CCA-4264-9E93-28ABC20F2B6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{CA583B3B-672B-499A-8D32-A8E7DEC0C921}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{CA583B3B-672B-499A-8D32-A8E7DEC0C921}"/>
   </bookViews>
   <sheets>
-    <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
+    <sheet name="tydzien 1" sheetId="1" r:id="rId1"/>
+    <sheet name="tydzien 2" sheetId="2" r:id="rId2"/>
+    <sheet name="tydzien 3" sheetId="3" r:id="rId3"/>
+    <sheet name="tydzien 4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -405,7 +408,51 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFE1757F-5429-4010-88EA-DF7AD98DC05C}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J34" sqref="J34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52BB998D-D26B-403A-93CE-CDB90AC601AC}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65DFB9E7-1B28-4C55-B124-62E362085D47}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K32" sqref="K32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E184EF9B-74F8-4BAC-B0F8-5903F6F0505E}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>

<commit_message>
utworzenie templatek w  backlogu
</commit_message>
<xml_diff>
--- a/backlog.xlsx
+++ b/backlog.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stasz\mistrz_klawiatury\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65C2F86E-0CCA-4264-9E93-28ABC20F2B6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA78C59F-8BEA-468D-9EA5-5A6B7DDC4FE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{CA583B3B-672B-499A-8D32-A8E7DEC0C921}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{CA583B3B-672B-499A-8D32-A8E7DEC0C921}"/>
   </bookViews>
   <sheets>
     <sheet name="tydzien 1" sheetId="1" r:id="rId1"/>
     <sheet name="tydzien 2" sheetId="2" r:id="rId2"/>
     <sheet name="tydzien 3" sheetId="3" r:id="rId3"/>
-    <sheet name="tydzien 4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,6 +35,29 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
+  <si>
+    <t>lp.</t>
+  </si>
+  <si>
+    <t>Kto wykonuje?</t>
+  </si>
+  <si>
+    <t>Priorytet</t>
+  </si>
+  <si>
+    <t>Zadanie- Sprint 1</t>
+  </si>
+  <si>
+    <t>Zadanie- Sprint 2</t>
+  </si>
+  <si>
+    <t>Zadanie- Sprint 3</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -87,6 +109,45 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B5F35E02-B7AF-4FBC-B2C5-A34190941716}" name="Tabela1" displayName="Tabela1" ref="A1:D18" totalsRowShown="0">
+  <autoFilter ref="A1:D18" xr:uid="{B5F35E02-B7AF-4FBC-B2C5-A34190941716}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{AF75DB00-49FB-43F3-ABE2-93EF7BA70B16}" name="lp."/>
+    <tableColumn id="2" xr3:uid="{F2E026D9-D2FE-4BC0-A38A-1156535E9BDB}" name="Zadanie- Sprint 1"/>
+    <tableColumn id="3" xr3:uid="{7805FABC-82DA-4540-82C0-D85A0E5E61DE}" name="Kto wykonuje?"/>
+    <tableColumn id="4" xr3:uid="{ED24A63D-8BB5-4E97-B1E5-D13FBFCF4C15}" name="Priorytet"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5D8D9B72-CA68-40D5-8872-0E1B433AD7FA}" name="Tabela13" displayName="Tabela13" ref="A1:D18" totalsRowShown="0">
+  <autoFilter ref="A1:D18" xr:uid="{5D8D9B72-CA68-40D5-8872-0E1B433AD7FA}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{5D1D9E52-F7EE-4A8F-93B2-7E997FC7801F}" name="lp."/>
+    <tableColumn id="2" xr3:uid="{F7ACE57C-2C44-45E4-BDF9-463E9A4F1D85}" name="Zadanie- Sprint 2"/>
+    <tableColumn id="3" xr3:uid="{A6B4CF38-EA9B-4A77-B47B-90AE03E28130}" name="Kto wykonuje?"/>
+    <tableColumn id="4" xr3:uid="{928FF769-F99D-4297-9BFC-BA43D32322F1}" name="Priorytet"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{99B028C5-2FC7-429C-94BB-558BCBDD2D7B}" name="Tabela14" displayName="Tabela14" ref="A1:D18" totalsRowShown="0">
+  <autoFilter ref="A1:D18" xr:uid="{99B028C5-2FC7-429C-94BB-558BCBDD2D7B}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{042E243D-A82D-44F0-B59C-E56D2B4A8958}" name="lp."/>
+    <tableColumn id="2" xr3:uid="{28785EAA-2DE0-466B-91F8-61F8BCE41011}" name="Zadanie- Sprint 3"/>
+    <tableColumn id="3" xr3:uid="{A26EC125-8138-498A-90BA-3CB1F6FA494D}" name="Kto wykonuje?"/>
+    <tableColumn id="4" xr3:uid="{8E5CC13D-58B0-45DB-BFBC-95751E0C2748}" name="Priorytet"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -406,56 +467,416 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFE1757F-5429-4010-88EA-DF7AD98DC05C}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J34" sqref="J34"/>
+      <selection activeCell="B26" activeCellId="1" sqref="A1:D18 B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="4.5703125" customWidth="1"/>
+    <col min="2" max="2" width="62" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f>A2+1</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f t="shared" ref="A4:A18" si="0">A3+1</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52BB998D-D26B-403A-93CE-CDB90AC601AC}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="42.42578125" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f>A2+1</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f t="shared" ref="A4:A18" si="0">A3+1</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65DFB9E7-1B28-4C55-B124-62E362085D47}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="4.85546875" customWidth="1"/>
+    <col min="2" max="2" width="52" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f>A2+1</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f t="shared" ref="A4:A18" si="0">A3+1</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E184EF9B-74F8-4BAC-B0F8-5903F6F0505E}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>